<commit_message>
Calculation and plot code split -- refactoring
</commit_message>
<xml_diff>
--- a/Model_Versions&Types.xlsx
+++ b/Model_Versions&Types.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Project\E555179_NAVIGATE\WP 6 - Documentation_Dissemination\6.3 Diagnostics paper\Analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7AF7CC-3471-4750-840D-97A875F7239A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3AB910-2F10-4CE9-8257-7516BF8466A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{CDF57776-780A-4DAC-ABE6-B3FC8F38F870}"/>
   </bookViews>
@@ -219,18 +219,6 @@
     <t>PE-RD</t>
   </si>
   <si>
-    <t>GE-IT</t>
-  </si>
-  <si>
-    <t>PE-IT</t>
-  </si>
-  <si>
-    <t>TIAM_Grantham_v3.2</t>
-  </si>
-  <si>
-    <t>TIAM_Grantham</t>
-  </si>
-  <si>
     <t>Policy Cost|Other</t>
   </si>
   <si>
@@ -247,6 +235,18 @@
   </si>
   <si>
     <t>GDP|PPP</t>
+  </si>
+  <si>
+    <t>PE-ITO</t>
+  </si>
+  <si>
+    <t>GE-ITO</t>
+  </si>
+  <si>
+    <t>TIAM-Grantham_v3.2</t>
+  </si>
+  <si>
+    <t>TIAM-Grantham</t>
   </si>
 </sst>
 </file>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037AF426-F990-4CAD-93E5-EC40FE7E59E8}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,7 +647,7 @@
         <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -670,7 +670,7 @@
         <v>56</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -693,7 +693,7 @@
         <v>56</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>52</v>
@@ -716,7 +716,7 @@
         <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="T4" s="2"/>
     </row>
@@ -731,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
         <v>53</v>
@@ -740,7 +740,7 @@
         <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
         <v>56</v>
       </c>
       <c r="G6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -786,7 +786,7 @@
         <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -809,7 +809,7 @@
         <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -832,7 +832,7 @@
         <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
         <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -878,7 +878,7 @@
         <v>56</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -901,7 +901,7 @@
         <v>56</v>
       </c>
       <c r="G12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -924,7 +924,7 @@
         <v>57</v>
       </c>
       <c r="G13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -947,7 +947,7 @@
         <v>56</v>
       </c>
       <c r="G14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -970,7 +970,7 @@
         <v>56</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -993,12 +993,12 @@
         <v>56</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>28</v>
@@ -1007,16 +1007,16 @@
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
         <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1030,7 +1030,7 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
         <v>51</v>
@@ -1039,7 +1039,7 @@
         <v>56</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
         <v>51</v>
@@ -1062,7 +1062,7 @@
         <v>56</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1076,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E20" t="s">
         <v>51</v>
@@ -1085,7 +1085,7 @@
         <v>56</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
         <v>56</v>
       </c>
       <c r="G21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1131,7 +1131,7 @@
         <v>56</v>
       </c>
       <c r="G22" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1154,7 +1154,7 @@
         <v>57</v>
       </c>
       <c r="G23" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1177,7 +1177,7 @@
         <v>57</v>
       </c>
       <c r="G24" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1191,7 +1191,7 @@
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E25" t="s">
         <v>51</v>
@@ -1200,7 +1200,7 @@
         <v>56</v>
       </c>
       <c r="G25" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1214,7 +1214,7 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E26" t="s">
         <v>51</v>
@@ -1223,7 +1223,7 @@
         <v>56</v>
       </c>
       <c r="G26" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1237,7 +1237,7 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E27" t="s">
         <v>51</v>
@@ -1246,30 +1246,30 @@
         <v>56</v>
       </c>
       <c r="G27" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" t="s">
-        <v>67</v>
-      </c>
       <c r="G28" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1283,7 +1283,7 @@
         <v>3</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E29" t="s">
         <v>53</v>
@@ -1292,7 +1292,7 @@
         <v>57</v>
       </c>
       <c r="G29" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1306,7 +1306,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E30" t="s">
         <v>53</v>
@@ -1315,7 +1315,7 @@
         <v>57</v>
       </c>
       <c r="G30" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1329,7 +1329,7 @@
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E31" t="s">
         <v>53</v>
@@ -1338,7 +1338,7 @@
         <v>57</v>
       </c>
       <c r="G31" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1352,7 +1352,7 @@
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E32" t="s">
         <v>51</v>
@@ -1361,7 +1361,7 @@
         <v>56</v>
       </c>
       <c r="G32" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1375,7 +1375,7 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E33" t="s">
         <v>51</v>
@@ -1384,7 +1384,7 @@
         <v>56</v>
       </c>
       <c r="G33" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>